<commit_message>
updates July 25 2020
</commit_message>
<xml_diff>
--- a/seeding/electric-guitars-seeding2.xlsx
+++ b/seeding/electric-guitars-seeding2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fremi-explorer2\seeding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B745F418-B195-43ED-8D4E-B1352BC8BC5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA79BC9D-9096-4EC0-A247-A6A1D970E5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCCB3FD7-56FB-44A7-8A7B-BD1E5D2B4346}"/>
   </bookViews>
@@ -7943,8 +7943,8 @@
   <dimension ref="A1:U569"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A173" sqref="A173"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>

</xml_diff>